<commit_message>
add pop up con info del tiempo de ejecucion
</commit_message>
<xml_diff>
--- a/src/lista_de_espias/lista-de-espias-larga.xlsx
+++ b/src/lista_de_espias/lista-de-espias-larga.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB2C6801-A30A-43BF-B7DF-41C8DABC27CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69D68BD8-56B5-4E02-BB33-AB0159293C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,6 +125,15 @@
     <t>0.23</t>
   </si>
   <si>
+    <t>Graciela</t>
+  </si>
+  <si>
+    <t>Lana</t>
+  </si>
+  <si>
+    <t>0.678</t>
+  </si>
+  <si>
     <t>Hugo</t>
   </si>
   <si>
@@ -149,6 +158,12 @@
     <t>0.95</t>
   </si>
   <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>0.212</t>
+  </si>
+  <si>
     <t>Jose</t>
   </si>
   <si>
@@ -176,6 +191,15 @@
     <t>Lucas</t>
   </si>
   <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
     <t>0.67</t>
   </si>
   <si>
@@ -215,9 +239,6 @@
     <t>0.98</t>
   </si>
   <si>
-    <t>0.64</t>
-  </si>
-  <si>
     <t>0.49</t>
   </si>
   <si>
@@ -260,15 +281,6 @@
     <t>0.99</t>
   </si>
   <si>
-    <t>Lana</t>
-  </si>
-  <si>
-    <t>0.001</t>
-  </si>
-  <si>
-    <t>0.85</t>
-  </si>
-  <si>
     <t>Simon</t>
   </si>
   <si>
@@ -278,19 +290,7 @@
     <t>0.21</t>
   </si>
   <si>
-    <t>Jorge</t>
-  </si>
-  <si>
     <t>0.002</t>
-  </si>
-  <si>
-    <t>Graciela</t>
-  </si>
-  <si>
-    <t>0.212</t>
-  </si>
-  <si>
-    <t>0.678</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C60" sqref="A2:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -853,10 +853,10 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
       <c r="C16" t="s">
@@ -864,91 +864,91 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
+      <c r="A17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" t="s">
-        <v>11</v>
+      <c r="A24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -956,10 +956,10 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -967,227 +967,227 @@
         <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>30</v>
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B31" t="s">
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
+      <c r="A35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>64</v>
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>28</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C43" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>9</v>
+      <c r="A44" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
       </c>
       <c r="C44" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C45" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>69</v>
-      </c>
-      <c r="B46" t="s">
-        <v>28</v>
       </c>
       <c r="C46" t="s">
         <v>72</v>
@@ -1195,98 +1195,98 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C47" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" t="s">
-        <v>19</v>
-      </c>
       <c r="C49" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C50" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C51" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C52" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s">
         <v>81</v>
@@ -1294,10 +1294,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C56" t="s">
         <v>82</v>
@@ -1305,32 +1305,32 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
         <v>83</v>
-      </c>
-      <c r="C57" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C58" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
         <v>86</v>
@@ -1338,18 +1338,18 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="C60" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C52">
-    <sortCondition ref="A2:A52"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+    <sortCondition ref="A2:A60"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>